<commit_message>
scraper for more pro players and data
</commit_message>
<xml_diff>
--- a/output/season_of_the_cat_2020.xlsx
+++ b/output/season_of_the_cat_2020.xlsx
@@ -58,7 +58,7 @@
     <t>Qnerr</t>
   </si>
   <si>
-    <t>hochu_kushat</t>
+    <t>yungxristcutwrist</t>
   </si>
   <si>
     <t>JSN991</t>
@@ -136,10 +136,10 @@
     <t>vendetta_sc</t>
   </si>
   <si>
-    <t>苏墨</t>
-  </si>
-  <si>
-    <t>21thCB</t>
+    <t>萌萌小西几</t>
+  </si>
+  <si>
+    <t>21stCB</t>
   </si>
   <si>
     <t>33Bogatyrya</t>
@@ -181,7 +181,7 @@
     <t>one_two12</t>
   </si>
   <si>
-    <t>xCyBerZz</t>
+    <t>xXxd4Rkk3V1nxXxD</t>
   </si>
   <si>
     <t>Pulisickness</t>
@@ -253,7 +253,7 @@
     <t>KusokStula</t>
   </si>
   <si>
-    <t>不再仁慈</t>
+    <t>解放</t>
   </si>
   <si>
     <t>elmundofrio</t>
@@ -316,7 +316,7 @@
     <t>Necrocyst</t>
   </si>
   <si>
-    <t>MisterLionov</t>
+    <t>Oblomov27</t>
   </si>
   <si>
     <t>Tamara_MT</t>
@@ -346,7 +346,7 @@
     <t>kakasi22</t>
   </si>
   <si>
-    <t>We_Will_Bury_You</t>
+    <t>ItsCommunismTime</t>
   </si>
   <si>
     <t>괴물을사랑하는사람</t>
@@ -439,7 +439,7 @@
     <t>Nequ1z</t>
   </si>
   <si>
-    <t>wangid3</t>
+    <t>五石散人</t>
   </si>
   <si>
     <t>Alex7Villa</t>
@@ -532,7 +532,7 @@
     <t>Kentoky84</t>
   </si>
   <si>
-    <t>pawlikus</t>
+    <t>ReynevanP</t>
   </si>
   <si>
     <t>Rieper137</t>
@@ -580,7 +580,7 @@
     <t>ALIMBAEV.ALIBEK</t>
   </si>
   <si>
-    <t>Lehudib</t>
+    <t>궨갤러</t>
   </si>
   <si>
     <t>toxanik</t>
@@ -664,7 +664,7 @@
     <t>SHEROS</t>
   </si>
   <si>
-    <t>Solnyshko1</t>
+    <t>SexyFallos</t>
   </si>
   <si>
     <t>King-T_3012</t>
@@ -820,7 +820,7 @@
     <t>haluton</t>
   </si>
   <si>
-    <t>psycho22</t>
+    <t>CaranthirOfAenElle</t>
   </si>
   <si>
     <t>Yurochichek</t>
@@ -838,7 +838,7 @@
     <t>Skyfreeman</t>
   </si>
   <si>
-    <t>RealLorenzOFFICIAL</t>
+    <t>PoppyCheeseburger</t>
   </si>
   <si>
     <t>macabrebump</t>
@@ -967,7 +967,7 @@
     <t>valdamon</t>
   </si>
   <si>
-    <t>_daruma</t>
+    <t>Koumakis</t>
   </si>
   <si>
     <t>Gogllum</t>
@@ -1126,7 +1126,7 @@
     <t>Sanctu5</t>
   </si>
   <si>
-    <t>我才是布列塔尼亞真正的王</t>
+    <t>砂糖精怪</t>
   </si>
   <si>
     <t>명상</t>
@@ -1192,7 +1192,7 @@
     <t>Sheath29</t>
   </si>
   <si>
-    <t>Quen123</t>
+    <t>Ken_0n</t>
   </si>
   <si>
     <t>Shukasa</t>
@@ -1291,7 +1291,7 @@
     <t>imSkry</t>
   </si>
   <si>
-    <t>GwentEnchanter</t>
+    <t>Eyesofapathy</t>
   </si>
   <si>
     <t>1stOfficer</t>
@@ -1489,7 +1489,7 @@
     <t>Vladimir_x</t>
   </si>
   <si>
-    <t>Dreghio</t>
+    <t>Akwarelista1888</t>
   </si>
   <si>
     <t>MongrelEyes</t>
@@ -1537,7 +1537,7 @@
     <t>valerinda1977</t>
   </si>
   <si>
-    <t>Sunday1972</t>
+    <t>LucjanK</t>
   </si>
   <si>
     <t>kamios</t>
@@ -1609,7 +1609,7 @@
     <t>Bad Atum</t>
   </si>
   <si>
-    <t>Fyrkalor</t>
+    <t>Satanly</t>
   </si>
   <si>
     <t>h1dd3n</t>
@@ -1648,13 +1648,13 @@
     <t>BEEFCAAAAKE</t>
   </si>
   <si>
-    <t>alozupone</t>
+    <t>penguinjunkie</t>
   </si>
   <si>
     <t>mayakori</t>
   </si>
   <si>
-    <t>DKM2493</t>
+    <t>Kabistan</t>
   </si>
   <si>
     <t>IIDox</t>
@@ -1666,10 +1666,10 @@
     <t>YngDanny</t>
   </si>
   <si>
-    <t>princemercury.17128</t>
-  </si>
-  <si>
-    <t>vezzi7890</t>
+    <t>秦皇岛精神岛民</t>
+  </si>
+  <si>
+    <t>Gw3ntPunk</t>
   </si>
   <si>
     <t>kamikaze13</t>
@@ -1711,7 +1711,7 @@
     <t>Mr.J.B-Man.ADC</t>
   </si>
   <si>
-    <t>9kjer</t>
+    <t>DziewiateSerce</t>
   </si>
   <si>
     <t>Feanor865</t>
@@ -1813,7 +1813,7 @@
     <t>BatGwent</t>
   </si>
   <si>
-    <t>你的笑容由我守护i</t>
+    <t>莫把湖面倒影当成夜空繁星</t>
   </si>
   <si>
     <t>Zanoza369246</t>
@@ -1870,7 +1870,7 @@
     <t>_RaVVaR_</t>
   </si>
   <si>
-    <t>Sovreign_95</t>
+    <t>Sovreign95</t>
   </si>
   <si>
     <t>happyGluk</t>
@@ -1894,7 +1894,7 @@
     <t>georgetruman</t>
   </si>
   <si>
-    <t>morelife44</t>
+    <t>-_V1PER_-</t>
   </si>
   <si>
     <t>Bl4ckHawk4</t>
@@ -1930,7 +1930,7 @@
     <t>molochss</t>
   </si>
   <si>
-    <t>Psycho-Pirate</t>
+    <t>Xurreus</t>
   </si>
   <si>
     <t>RedShagreen</t>
@@ -1954,7 +1954,7 @@
     <t>exhaust_pipe</t>
   </si>
   <si>
-    <t>pepsikolniy228</t>
+    <t>pepsikolniy_228_</t>
   </si>
   <si>
     <t>romeys</t>
@@ -1969,7 +1969,7 @@
     <t>acbmn113</t>
   </si>
   <si>
-    <t>nvcz</t>
+    <t>MaradonaEterno</t>
   </si>
   <si>
     <t>MATPOC_JlOM</t>
@@ -1984,7 +1984,7 @@
     <t>Erdoganishe2</t>
   </si>
   <si>
-    <t>岸边露伴上蹿下跳</t>
+    <t>退堂鼓小能手</t>
   </si>
   <si>
     <t>ehufof13</t>
@@ -2062,7 +2062,7 @@
     <t>1ceArr0w</t>
   </si>
   <si>
-    <t>Sir_Drew_Solo</t>
+    <t>Hawgplex</t>
   </si>
   <si>
     <t>Count-Dooku</t>
@@ -2191,7 +2191,7 @@
     <t>Varioo</t>
   </si>
   <si>
-    <t>三笠是个萌妹纸</t>
+    <t>枫和sama</t>
   </si>
   <si>
     <t>Dimernyte</t>
@@ -2263,7 +2263,7 @@
     <t>SoltysZadupia</t>
   </si>
   <si>
-    <t>Bartek_Nowicki</t>
+    <t>Gaunter_O_Clock</t>
   </si>
   <si>
     <t>youkohige</t>
@@ -2281,7 +2281,7 @@
     <t>7evev</t>
   </si>
   <si>
-    <t>rayzz4</t>
+    <t>云游rayzz4</t>
   </si>
   <si>
     <t>Sergey_Ka</t>
@@ -2449,7 +2449,7 @@
     <t>TN_jamedi</t>
   </si>
   <si>
-    <t>Arachnne</t>
+    <t>Angoul3me</t>
   </si>
   <si>
     <t>魔法少女叶奈法</t>
@@ -2644,7 +2644,7 @@
     <t>5Ares5</t>
   </si>
   <si>
-    <t>Gwent867</t>
+    <t>PATRIOT.3.6.9</t>
   </si>
   <si>
     <t>PaxRomana395</t>
@@ -2677,7 +2677,7 @@
     <t>paw68kis</t>
   </si>
   <si>
-    <t>JU_STER</t>
+    <t>4EiZ</t>
   </si>
   <si>
     <t>23JD23</t>
@@ -2860,7 +2860,7 @@
     <t>tocacu</t>
   </si>
   <si>
-    <t>iluxa228</t>
+    <t>BigKukuRUzina35</t>
   </si>
   <si>
     <t>DT-nl</t>
@@ -2869,7 +2869,7 @@
     <t>IronColt</t>
   </si>
   <si>
-    <t>dakorika</t>
+    <t>Dakoriko</t>
   </si>
   <si>
     <t>Krypton77777</t>
@@ -2887,7 +2887,7 @@
     <t>Niv2123</t>
   </si>
   <si>
-    <t>romanyartsev</t>
+    <t>Son_of_Spardaa</t>
   </si>
   <si>
     <t>SChungy</t>
@@ -3043,7 +3043,7 @@
     <t>1KOLOSS1</t>
   </si>
   <si>
-    <t>Bastion99</t>
+    <t>Karasmai</t>
   </si>
   <si>
     <t>Pacifier3750</t>
@@ -3133,7 +3133,7 @@
     <t>やり手のあきら</t>
   </si>
   <si>
-    <t>bGyZ</t>
+    <t>be_gyz</t>
   </si>
   <si>
     <t>SiRgr3x</t>
@@ -3319,7 +3319,7 @@
     <t>你可知我</t>
   </si>
   <si>
-    <t>荼荼LAN子</t>
+    <t>hLanZi</t>
   </si>
   <si>
     <t>Trung200888</t>
@@ -3337,7 +3337,7 @@
     <t>Raskyu</t>
   </si>
   <si>
-    <t>W.Rooney</t>
+    <t>帝国大金</t>
   </si>
   <si>
     <t>hoori1</t>
@@ -3397,7 +3397,7 @@
     <t>MatZzoo</t>
   </si>
   <si>
-    <t>Luxwang</t>
+    <t>用微笑书写无奈</t>
   </si>
   <si>
     <t>CstFox</t>
@@ -3616,7 +3616,7 @@
     <t>Dark_Solo</t>
   </si>
   <si>
-    <t>Astralis丶</t>
+    <t>gla1ve丶</t>
   </si>
   <si>
     <t>fener2100</t>
@@ -3739,7 +3739,7 @@
     <t>Nerosyrian44</t>
   </si>
   <si>
-    <t>윤동빈</t>
+    <t>일상생활가능한가요</t>
   </si>
   <si>
     <t>l_PeChKa_l</t>
@@ -3763,7 +3763,7 @@
     <t>lilounator</t>
   </si>
   <si>
-    <t>正十七</t>
+    <t>埃斯特庄园的喷泉</t>
   </si>
   <si>
     <t>Avrillax</t>
@@ -3826,7 +3826,7 @@
     <t>pakyleone90</t>
   </si>
   <si>
-    <t>TA_JMJWilson</t>
+    <t>JMJWilson23</t>
   </si>
   <si>
     <t>McSwaggin</t>
@@ -3922,7 +3922,7 @@
     <t>Ambiral</t>
   </si>
   <si>
-    <t>Tragic_Bronson</t>
+    <t>Miskuzi_</t>
   </si>
   <si>
     <t>MoonTalonRaven</t>
@@ -4057,7 +4057,7 @@
     <t>AlasdairCampbell85</t>
   </si>
   <si>
-    <t>vktr_vktr</t>
+    <t>T-3OOO</t>
   </si>
   <si>
     <t>Jammomcd</t>
@@ -4066,7 +4066,7 @@
     <t>Gerry76</t>
   </si>
   <si>
-    <t>LaRespuesta</t>
+    <t>T-MacforMVP</t>
   </si>
   <si>
     <t>ISILDURRRR</t>
@@ -4102,7 +4102,7 @@
     <t>Drmustachein</t>
   </si>
   <si>
-    <t>IIpoxBocT</t>
+    <t>YaDart</t>
   </si>
   <si>
     <t>Exanthemas</t>
@@ -4162,7 +4162,7 @@
     <t>布兰德奇</t>
   </si>
   <si>
-    <t>Xin_Juin</t>
+    <t>bananapotato818</t>
   </si>
   <si>
     <t>ArryR</t>
@@ -4189,7 +4189,7 @@
     <t>Mazzai</t>
   </si>
   <si>
-    <t>SeventyThreeB</t>
+    <t>PeepoGlad</t>
   </si>
   <si>
     <t>Pain1pain</t>
@@ -4255,7 +4255,7 @@
     <t>Valuuy</t>
   </si>
   <si>
-    <t>2357906099</t>
+    <t>X黎星X</t>
   </si>
   <si>
     <t>kopli23</t>
@@ -4288,7 +4288,7 @@
     <t>Hokey-Pokey</t>
   </si>
   <si>
-    <t>Lazheer</t>
+    <t>AstoraKnight</t>
   </si>
   <si>
     <t>xLuxa4x</t>
@@ -4330,7 +4330,7 @@
     <t>Brak_Formy</t>
   </si>
   <si>
-    <t>Marbi124</t>
+    <t>Bard_Martin</t>
   </si>
   <si>
     <t>Andrjuxaxa</t>
@@ -4354,7 +4354,7 @@
     <t>Unfortunate.</t>
   </si>
   <si>
-    <t>batmanzero</t>
+    <t>BAT0MAN</t>
   </si>
   <si>
     <t>Excelshortloin</t>
@@ -4447,7 +4447,7 @@
     <t>Matteo2497</t>
   </si>
   <si>
-    <t>MastiGame</t>
+    <t>Domm92</t>
   </si>
   <si>
     <t>IpolserI</t>
@@ -4462,7 +4462,7 @@
     <t>Sohnareli</t>
   </si>
   <si>
-    <t>PepegaFF</t>
+    <t>alkso_junior</t>
   </si>
   <si>
     <t>duguhao123</t>
@@ -4558,7 +4558,7 @@
     <t>AlexNorton228</t>
   </si>
   <si>
-    <t>Charalambos_Ioanno</t>
+    <t>Chambos101</t>
   </si>
   <si>
     <t>Raimee</t>
@@ -4630,7 +4630,7 @@
     <t>Olegicus</t>
   </si>
   <si>
-    <t>siechahot</t>
+    <t>Lt_Marsh</t>
   </si>
   <si>
     <t>hajcik1</t>
@@ -4681,7 +4681,7 @@
     <t>damarques</t>
   </si>
   <si>
-    <t>WildB0ar</t>
+    <t>L9ettal</t>
   </si>
   <si>
     <t>bocadexunana</t>
@@ -4876,7 +4876,7 @@
     <t>Paiki</t>
   </si>
   <si>
-    <t>DarthLothins</t>
+    <t>darthlothins</t>
   </si>
   <si>
     <t>qturtle87</t>
@@ -5071,7 +5071,7 @@
     <t>bratrJen</t>
   </si>
   <si>
-    <t>magistrkiller</t>
+    <t>m_1_s_T</t>
   </si>
   <si>
     <t>Giobo</t>
@@ -5335,7 +5335,7 @@
     <t>The_Spriggan</t>
   </si>
   <si>
-    <t>lSolist</t>
+    <t>PASHAZOREdd__</t>
   </si>
   <si>
     <t>Dustyspore313</t>
@@ -5347,7 +5347,7 @@
     <t>Mem_OG</t>
   </si>
   <si>
-    <t>ChidiAnagonye</t>
+    <t>SirAdamPadam</t>
   </si>
   <si>
     <t>K3lla</t>
@@ -5497,7 +5497,7 @@
     <t>JWilliamJames</t>
   </si>
   <si>
-    <t>四木团子</t>
+    <t>与艾莉欧团长在秋天的单相思</t>
   </si>
   <si>
     <t>Kn1azev</t>
@@ -5551,7 +5551,7 @@
     <t>黑橙子</t>
   </si>
   <si>
-    <t>DED_MOROZ29</t>
+    <t>yakymenko29</t>
   </si>
   <si>
     <t>W_Flume</t>
@@ -5563,7 +5563,7 @@
     <t>EmGie_Grzywna</t>
   </si>
   <si>
-    <t>kypec-bakaleyshik</t>
+    <t>sfqwe</t>
   </si>
   <si>
     <t>Semirt</t>
@@ -5602,7 +5602,7 @@
     <t>Neves_Kaos</t>
   </si>
   <si>
-    <t>nilfbojest</t>
+    <t>3zform3</t>
   </si>
   <si>
     <t>NIKEMEN</t>
@@ -5629,7 +5629,7 @@
     <t>wyc345</t>
   </si>
   <si>
-    <t>阿暐</t>
+    <t>阿纬</t>
   </si>
   <si>
     <t>Dimetz1</t>
@@ -5662,7 +5662,7 @@
     <t>RU_Heavy</t>
   </si>
   <si>
-    <t>Casper_01</t>
+    <t>_C4SPER</t>
   </si>
   <si>
     <t>巫师三限时原价又结束了</t>
@@ -5857,7 +5857,7 @@
     <t>brook.80027</t>
   </si>
   <si>
-    <t>JanBergen</t>
+    <t>LeoWhiteFang</t>
   </si>
   <si>
     <t>ZussyQ</t>
@@ -5935,7 +5935,7 @@
     <t>sacroon</t>
   </si>
   <si>
-    <t>fak_off</t>
+    <t>PatienceNotAVirtue</t>
   </si>
   <si>
     <t>Uncle-Dutch</t>
@@ -6298,7 +6298,7 @@
     <t>Gerasimchuk</t>
   </si>
   <si>
-    <t>GwentTeamDestroyer</t>
+    <t>gniloycowboy</t>
   </si>
   <si>
     <t>Shopot131415</t>
@@ -6490,7 +6490,7 @@
     <t>Hirota6</t>
   </si>
   <si>
-    <t>AlexZhdan</t>
+    <t>Uzzbek</t>
   </si>
   <si>
     <t>Johnsonzxc</t>
@@ -6517,7 +6517,7 @@
     <t>Rybana</t>
   </si>
   <si>
-    <t>SilverSkadi_</t>
+    <t>SilverSwallow</t>
   </si>
   <si>
     <t>vardges</t>
@@ -6619,7 +6619,7 @@
     <t>Detalis</t>
   </si>
   <si>
-    <t>KIRALZC</t>
+    <t>CCPTheCNGang</t>
   </si>
   <si>
     <t>Silllenzio</t>
@@ -6634,13 +6634,13 @@
     <t>Ganillik</t>
   </si>
   <si>
-    <t>Deremosh</t>
+    <t>Lord_Parsifal</t>
   </si>
   <si>
     <t>Dekenn</t>
   </si>
   <si>
-    <t>ertzu78</t>
+    <t>RustyDynamo</t>
   </si>
   <si>
     <t>Alurklin</t>
@@ -7207,7 +7207,7 @@
     <t>HarryLooockhart</t>
   </si>
   <si>
-    <t>lpwwww5</t>
+    <t>月移花影上栏杆</t>
   </si>
   <si>
     <t>Jopa26</t>
@@ -7234,7 +7234,7 @@
     <t>Ahnitho</t>
   </si>
   <si>
-    <t>Demonisimo</t>
+    <t>NilfFunGirl</t>
   </si>
   <si>
     <t>HssScooter</t>
@@ -7324,13 +7324,13 @@
     <t>-Arrowhead-</t>
   </si>
   <si>
-    <t>PuppetCrow</t>
+    <t>Liliedcat</t>
   </si>
   <si>
     <t>thesolidstate</t>
   </si>
   <si>
-    <t>徐北游</t>
+    <t>发牌员真是个小天才</t>
   </si>
   <si>
     <t>par_chin_10</t>
@@ -7363,16 +7363,16 @@
     <t>JeeWent</t>
   </si>
   <si>
-    <t>MarkoPolloCD</t>
-  </si>
-  <si>
-    <t>再也不打昆特牌了</t>
+    <t>SweetBirdy</t>
+  </si>
+  <si>
+    <t>我自纵横</t>
   </si>
   <si>
     <t>SkavarodkerTM</t>
   </si>
   <si>
-    <t>rfcvp</t>
+    <t>fan_of_clann</t>
   </si>
   <si>
     <t>希里.</t>
@@ -7459,10 +7459,10 @@
     <t>Crockse</t>
   </si>
   <si>
-    <t>천우희희희</t>
-  </si>
-  <si>
-    <t>Verusul</t>
+    <t>신세휘</t>
+  </si>
+  <si>
+    <t>RaggamuffinEZ</t>
   </si>
   <si>
     <t>Ardetho</t>
@@ -7531,13 +7531,13 @@
     <t>Diesel-rd</t>
   </si>
   <si>
-    <t>ArtemAB</t>
+    <t>PatriotUA58</t>
   </si>
   <si>
     <t>ZipPeLl</t>
   </si>
   <si>
-    <t>Sanyasanya</t>
+    <t>Mr_Redboy</t>
   </si>
   <si>
     <t>Ka3yucm</t>
@@ -7558,7 +7558,7 @@
     <t>Kisky</t>
   </si>
   <si>
-    <t>Splazyy</t>
+    <t>contascy</t>
   </si>
   <si>
     <t>Sean6620</t>
@@ -7594,7 +7594,7 @@
     <t>PigmanTM</t>
   </si>
   <si>
-    <t>josephoakenshield</t>
+    <t>游天神龙</t>
   </si>
   <si>
     <t>Barni420</t>
@@ -7702,7 +7702,7 @@
     <t>Zannihk</t>
   </si>
   <si>
-    <t>无心.68680</t>
+    <t>老子才是无心</t>
   </si>
   <si>
     <t>Koshak1538</t>
@@ -7738,7 +7738,7 @@
     <t>ben_148</t>
   </si>
   <si>
-    <t>KingWeasel84</t>
+    <t>JackBauer84</t>
   </si>
   <si>
     <t>RECD</t>
@@ -7756,7 +7756,7 @@
     <t>Vientos89</t>
   </si>
   <si>
-    <t>TheMidnightStalker</t>
+    <t>TheMeditator</t>
   </si>
   <si>
     <t>Norbsky</t>
@@ -7786,7 +7786,7 @@
     <t>YURA_RAKETA</t>
   </si>
   <si>
-    <t>jesulete</t>
+    <t>Maurandi</t>
   </si>
   <si>
     <t>Mavzes</t>
@@ -7867,7 +7867,7 @@
     <t>防火阀照镜子</t>
   </si>
   <si>
-    <t>牛丝屯</t>
+    <t>牛四屯</t>
   </si>
   <si>
     <t>Kuzzzzzia</t>
@@ -7936,7 +7936,7 @@
     <t>Papannn9</t>
   </si>
   <si>
-    <t>零ZER0</t>
+    <t>Bulgarus</t>
   </si>
   <si>
     <t>PHANATIC82</t>
@@ -7951,7 +7951,7 @@
     <t>Хипи</t>
   </si>
   <si>
-    <t>DonFurion</t>
+    <t>NOVAQ88</t>
   </si>
   <si>
     <t>maYEStro1337</t>
@@ -8044,7 +8044,7 @@
     <t>King-Puck</t>
   </si>
   <si>
-    <t>PUYLO</t>
+    <t>ProPeaceDon</t>
   </si>
   <si>
     <t>Radiantfull</t>
@@ -8338,7 +8338,7 @@
     <t>amramajeed</t>
   </si>
   <si>
-    <t>Kamenriders</t>
+    <t>Lotteria88</t>
   </si>
   <si>
     <t>koke16</t>
@@ -8431,7 +8431,7 @@
     <t>RixTrixx</t>
   </si>
   <si>
-    <t>jvstnp</t>
+    <t>JVSTN</t>
   </si>
   <si>
     <t>ScorchThePeasant</t>
@@ -8524,7 +8524,7 @@
     <t>Pawlas12757</t>
   </si>
   <si>
-    <t>Bostjan_Brumec</t>
+    <t>Bo_Br</t>
   </si>
   <si>
     <t>KiViN_777</t>
@@ -8572,7 +8572,7 @@
     <t>LarbPed</t>
   </si>
   <si>
-    <t>adnume</t>
+    <t>trissocute</t>
   </si>
   <si>
     <t>阳神虚度</t>

</xml_diff>